<commit_message>
optimization_diagnostic is created whenever we estimate the parameters.
</commit_message>
<xml_diff>
--- a/test_files/estimation_tests/3-genes_3-edges_artificial-data_Sigmoid_estimation_1.xlsx
+++ b/test_files/estimation_tests/3-genes_3-edges_artificial-data_Sigmoid_estimation_1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="644" activeTab="6"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20610" windowHeight="11640" tabRatio="644" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="production_rates" sheetId="13" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>alpha</t>
   </si>
@@ -32,27 +32,12 @@
     <t>kk_max</t>
   </si>
   <si>
-    <t>SystematicName</t>
-  </si>
-  <si>
-    <t>StandardName</t>
-  </si>
-  <si>
-    <t>DegradationRate</t>
-  </si>
-  <si>
-    <t>rows genes affected/cols genes controlling</t>
-  </si>
-  <si>
     <t>value</t>
   </si>
   <si>
     <t>optimization_parameter</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>MaxIter</t>
   </si>
   <si>
@@ -65,9 +50,6 @@
     <t>TolX</t>
   </si>
   <si>
-    <t>production_rates</t>
-  </si>
-  <si>
     <t>Strain</t>
   </si>
   <si>
@@ -89,24 +71,12 @@
     <t>Sigmoid</t>
   </si>
   <si>
-    <t>simtime</t>
-  </si>
-  <si>
-    <t>sysGene1</t>
-  </si>
-  <si>
     <t>QT1</t>
   </si>
   <si>
-    <t>sysGene2</t>
-  </si>
-  <si>
     <t>SMRT1</t>
   </si>
   <si>
-    <t>sysGene3</t>
-  </si>
-  <si>
     <t>WRD2</t>
   </si>
   <si>
@@ -116,20 +86,45 @@
     <t>run with fixed b (all 0) and fixed P the result should be optimized weights in absolute value less than tolX</t>
   </si>
   <si>
-    <t>estimateParams</t>
-  </si>
-  <si>
-    <t>makeGraphs</t>
+    <t>estimate_params</t>
+  </si>
+  <si>
+    <t>make_graphs</t>
+  </si>
+  <si>
+    <t>expression_timepoints</t>
+  </si>
+  <si>
+    <t>simulation_timepoints</t>
+  </si>
+  <si>
+    <t>production_rate</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>degradation_rate</t>
+  </si>
+  <si>
+    <t>regulators/controllers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -163,23 +158,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,186 +546,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
-      <c r="H1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="H2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4">
         <v>1.6</v>
       </c>
-      <c r="H3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="H4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D4" s="5"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5" s="4"/>
-      <c r="E5" s="5"/>
-      <c r="H5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-      <c r="H6"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-      <c r="H9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-      <c r="H11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-      <c r="H12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-      <c r="E13" s="5"/>
-      <c r="H13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-      <c r="H14"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-      <c r="H15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-      <c r="H16"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-      <c r="H17"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-      <c r="H18"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19"/>
-      <c r="B19"/>
-      <c r="C19" s="4"/>
-      <c r="E19" s="5"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" s="4"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
-      <c r="H22"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="5"/>
+      <c r="G22"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -734,153 +703,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="B2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="4">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4">
         <v>0.8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12"/>
-      <c r="B12"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17"/>
-      <c r="B17"/>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19"/>
       <c r="B19"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20"/>
       <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21"/>
       <c r="B21"/>
-      <c r="C21"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22"/>
       <c r="B22"/>
-      <c r="C22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -892,67 +830,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="7">
+        <v>25</v>
+      </c>
+      <c r="B1" s="6">
         <v>5</v>
       </c>
-      <c r="D1" s="7">
+      <c r="C1" s="6">
         <v>5</v>
       </c>
-      <c r="E1" s="7">
+      <c r="D1" s="6">
         <v>5</v>
       </c>
-      <c r="F1" s="7">
+      <c r="E1" s="6">
         <v>5</v>
       </c>
-      <c r="G1" s="7">
+      <c r="F1" s="6">
         <v>10</v>
       </c>
-      <c r="H1" s="7">
+      <c r="G1" s="6">
         <v>10</v>
       </c>
-      <c r="I1" s="7">
+      <c r="H1" s="6">
         <v>10</v>
       </c>
-      <c r="J1" s="7">
+      <c r="I1" s="6">
         <v>10</v>
       </c>
-      <c r="K1" s="7">
+      <c r="J1" s="6">
         <v>20</v>
       </c>
-      <c r="L1" s="7">
+      <c r="K1" s="6">
         <v>20</v>
       </c>
-      <c r="M1" s="7">
+      <c r="L1" s="6">
         <v>20</v>
       </c>
-      <c r="N1" s="7">
+      <c r="M1" s="6">
         <v>20</v>
       </c>
-      <c r="O1" s="7">
+      <c r="N1" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -990,16 +925,13 @@
       <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1037,16 +969,13 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1084,43 +1013,40 @@
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G6" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G12" s="2"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="I14" s="2"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="I18" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F20" s="2"/>
-      <c r="M20" s="2"/>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="L20" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -1130,9 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1157,22 +1081,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
+      <c r="A1" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -1186,7 +1110,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1200,7 +1124,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1224,9 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1250,17 +1172,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>5</v>
+      <c r="A1" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E1"/>
       <c r="F1"/>
@@ -1283,7 +1205,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B2" s="4">
         <v>0.1</v>
@@ -1297,7 +1219,7 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1311,7 +1233,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1324,7 +1246,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -1336,7 +1258,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1346,26 +1268,26 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
@@ -1373,7 +1295,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -1381,82 +1303,82 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
+      <c r="A4" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
+      <c r="A5" s="11" t="s">
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
+      <c r="A6" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>1000000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
+      <c r="A7" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>31</v>
+      <c r="A10" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="9">
+      <c r="A13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="8">
         <v>5</v>
       </c>
       <c r="C13">
@@ -1467,32 +1389,32 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>14</v>
+      <c r="A14" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="8">
+      <c r="A15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8">
+      <c r="A16" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>21</v>
+      <c r="A17" s="11" t="s">
+        <v>23</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1570,20 +1492,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>5</v>
+      <c r="A1" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1591,7 +1511,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1599,7 +1519,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -1612,7 +1532,7 @@
       <c r="A17" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1621,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1629,12 +1549,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>